<commit_message>
working on updating unknown frag IDs
</commit_message>
<xml_diff>
--- a/data/PAM_metadata.xlsx
+++ b/data/PAM_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/GT23_Heat_Microbiome/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shayle/Desktop/Projects/GT23_Heat_Microbiome/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFFC0D5-A074-5C4C-B602-7036DD946E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFAE3F0-0D81-E748-9FA8-8CEB48F521AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="500" windowWidth="21360" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-840" yWindow="460" windowWidth="21360" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="104">
   <si>
     <t>Date:</t>
   </si>
@@ -92,9 +92,6 @@
     <t>1281-11</t>
   </si>
   <si>
-    <t>1273-4(or 11)</t>
-  </si>
-  <si>
     <t>or -11</t>
   </si>
   <si>
@@ -149,22 +146,13 @@
     <t>874-11</t>
   </si>
   <si>
-    <t>129-11</t>
-  </si>
-  <si>
     <t>873-2</t>
-  </si>
-  <si>
-    <t>128-7</t>
   </si>
   <si>
     <t>1291-2</t>
   </si>
   <si>
     <t>1292-2</t>
-  </si>
-  <si>
-    <t>128-6</t>
   </si>
   <si>
     <t>1235-8</t>
@@ -206,9 +194,6 @@
     <t>1281-3</t>
   </si>
   <si>
-    <t>127-7</t>
-  </si>
-  <si>
     <t>1283-4</t>
   </si>
   <si>
@@ -222,9 +207,6 @@
   </si>
   <si>
     <t>1271-5</t>
-  </si>
-  <si>
-    <t>871-7</t>
   </si>
   <si>
     <t>873-3</t>
@@ -272,9 +254,6 @@
     <t>873-11</t>
   </si>
   <si>
-    <t>123-9</t>
-  </si>
-  <si>
     <t>1273-11</t>
   </si>
   <si>
@@ -302,15 +281,6 @@
     <t>12??-11</t>
   </si>
   <si>
-    <t>824-8</t>
-  </si>
-  <si>
-    <t>87?-7</t>
-  </si>
-  <si>
-    <t>127?-7</t>
-  </si>
-  <si>
     <t>872-11</t>
   </si>
   <si>
@@ -330,9 +300,6 @@
   </si>
   <si>
     <t>128?-8</t>
-  </si>
-  <si>
-    <t>127X-7</t>
   </si>
   <si>
     <t>12XX-2</t>
@@ -375,6 +342,9 @@
   </si>
   <si>
     <t>1281-6</t>
+  </si>
+  <si>
+    <t>1271-4 or 1273-2</t>
   </si>
 </sst>
 </file>
@@ -431,7 +401,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -719,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -729,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A654" workbookViewId="0">
-      <selection activeCell="D685" sqref="D685"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="194" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1285,7 +1255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>45061</v>
       </c>
@@ -1302,7 +1272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>45061</v>
       </c>
@@ -1319,7 +1289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>45061</v>
       </c>
@@ -1336,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>45061</v>
       </c>
@@ -1353,7 +1323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>45061</v>
       </c>
@@ -1370,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45061</v>
       </c>
@@ -1387,7 +1357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>45061</v>
       </c>
@@ -1404,7 +1374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>45061</v>
       </c>
@@ -1421,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>45061</v>
       </c>
@@ -1438,7 +1408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45061</v>
       </c>
@@ -1449,16 +1419,13 @@
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="E42">
         <v>3</v>
       </c>
-      <c r="F42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>45061</v>
       </c>
@@ -1469,13 +1436,13 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E43">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45061</v>
       </c>
@@ -1486,13 +1453,13 @@
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E44">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>45061</v>
       </c>
@@ -1509,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45061</v>
       </c>
@@ -1526,7 +1493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45061</v>
       </c>
@@ -1543,7 +1510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45061</v>
       </c>
@@ -1577,7 +1544,7 @@
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1659,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -1676,7 +1643,7 @@
         <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -1693,7 +1660,7 @@
         <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E56">
         <v>3</v>
@@ -1710,7 +1677,7 @@
         <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -1727,7 +1694,7 @@
         <v>12</v>
       </c>
       <c r="D58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E58">
         <v>5</v>
@@ -1744,7 +1711,7 @@
         <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E59">
         <v>6</v>
@@ -1761,7 +1728,7 @@
         <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E60">
         <v>7</v>
@@ -1795,7 +1762,7 @@
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -1812,7 +1779,7 @@
         <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E63">
         <v>3</v>
@@ -1829,13 +1796,13 @@
         <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E64">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>45061</v>
       </c>
@@ -1852,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>45061</v>
       </c>
@@ -1869,7 +1836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>45061</v>
       </c>
@@ -1886,7 +1853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>45061</v>
       </c>
@@ -1903,7 +1870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>45061</v>
       </c>
@@ -1920,7 +1887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>45061</v>
       </c>
@@ -1937,7 +1904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>45061</v>
       </c>
@@ -1954,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>45061</v>
       </c>
@@ -1971,7 +1938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>45061</v>
       </c>
@@ -1988,7 +1955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>45061</v>
       </c>
@@ -2005,7 +1972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>45061</v>
       </c>
@@ -2016,13 +1983,13 @@
         <v>16</v>
       </c>
       <c r="D75" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E75">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>45061</v>
       </c>
@@ -2033,16 +2000,13 @@
         <v>16</v>
       </c>
       <c r="D76" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E76">
         <v>2</v>
       </c>
-      <c r="F76" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>45061</v>
       </c>
@@ -2053,13 +2017,13 @@
         <v>16</v>
       </c>
       <c r="D77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E77">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>45061</v>
       </c>
@@ -2070,16 +2034,13 @@
         <v>16</v>
       </c>
       <c r="D78" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E78">
         <v>4</v>
       </c>
-      <c r="F78" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>45061</v>
       </c>
@@ -2090,13 +2051,13 @@
         <v>16</v>
       </c>
       <c r="D79" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E79">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>45061</v>
       </c>
@@ -2107,13 +2068,10 @@
         <v>17</v>
       </c>
       <c r="D80" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="E80">
         <v>1</v>
-      </c>
-      <c r="F80" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2127,7 +2085,7 @@
         <v>17</v>
       </c>
       <c r="D81" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E81">
         <v>2</v>
@@ -2144,10 +2102,13 @@
         <v>17</v>
       </c>
       <c r="D82" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E82">
         <v>3</v>
+      </c>
+      <c r="F82" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2161,13 +2122,10 @@
         <v>17</v>
       </c>
       <c r="D83" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="E83">
         <v>4</v>
-      </c>
-      <c r="F83" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2181,10 +2139,13 @@
         <v>17</v>
       </c>
       <c r="D84" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E84">
         <v>5</v>
+      </c>
+      <c r="F84" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2385,7 +2346,7 @@
         <v>20</v>
       </c>
       <c r="D96" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -2402,7 +2363,7 @@
         <v>20</v>
       </c>
       <c r="D97" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E97">
         <v>2</v>
@@ -2419,7 +2380,7 @@
         <v>20</v>
       </c>
       <c r="D98" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E98">
         <v>3</v>
@@ -2436,7 +2397,7 @@
         <v>20</v>
       </c>
       <c r="D99" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E99">
         <v>4</v>
@@ -2453,7 +2414,7 @@
         <v>20</v>
       </c>
       <c r="D100" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E100">
         <v>5</v>
@@ -2470,7 +2431,7 @@
         <v>21</v>
       </c>
       <c r="D101" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -2487,7 +2448,7 @@
         <v>21</v>
       </c>
       <c r="D102" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E102">
         <v>2</v>
@@ -2504,7 +2465,7 @@
         <v>21</v>
       </c>
       <c r="D103" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E103">
         <v>3</v>
@@ -2521,7 +2482,7 @@
         <v>21</v>
       </c>
       <c r="D104" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E104">
         <v>4</v>
@@ -2538,13 +2499,13 @@
         <v>21</v>
       </c>
       <c r="D105" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E105">
         <v>5</v>
       </c>
       <c r="F105" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -2558,7 +2519,7 @@
         <v>22</v>
       </c>
       <c r="D106" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -2575,7 +2536,7 @@
         <v>22</v>
       </c>
       <c r="D107" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E107">
         <v>2</v>
@@ -2592,13 +2553,10 @@
         <v>22</v>
       </c>
       <c r="D108" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="E108">
         <v>3</v>
-      </c>
-      <c r="F108" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -2612,7 +2570,7 @@
         <v>22</v>
       </c>
       <c r="D109" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E109">
         <v>4</v>
@@ -2629,7 +2587,7 @@
         <v>22</v>
       </c>
       <c r="D110" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E110">
         <v>5</v>
@@ -2646,7 +2604,7 @@
         <v>22</v>
       </c>
       <c r="D111" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E111">
         <v>6</v>
@@ -2663,7 +2621,7 @@
         <v>22</v>
       </c>
       <c r="D112" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E112">
         <v>7</v>
@@ -2680,7 +2638,7 @@
         <v>23</v>
       </c>
       <c r="D113" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -2697,7 +2655,7 @@
         <v>23</v>
       </c>
       <c r="D114" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E114">
         <v>2</v>
@@ -2714,7 +2672,7 @@
         <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E115">
         <v>3</v>
@@ -2731,7 +2689,7 @@
         <v>23</v>
       </c>
       <c r="D116" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E116">
         <v>4</v>
@@ -2748,7 +2706,7 @@
         <v>23</v>
       </c>
       <c r="D117" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E117">
         <v>5</v>
@@ -2765,7 +2723,7 @@
         <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E118">
         <v>6</v>
@@ -2782,7 +2740,7 @@
         <v>23</v>
       </c>
       <c r="D119" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E119">
         <v>7</v>
@@ -2918,7 +2876,7 @@
         <v>25</v>
       </c>
       <c r="D127" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E127">
         <v>4</v>
@@ -2969,7 +2927,7 @@
         <v>26</v>
       </c>
       <c r="D130" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -2986,7 +2944,7 @@
         <v>26</v>
       </c>
       <c r="D131" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E131">
         <v>2</v>
@@ -3003,7 +2961,7 @@
         <v>26</v>
       </c>
       <c r="D132" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E132">
         <v>3</v>
@@ -3020,7 +2978,7 @@
         <v>26</v>
       </c>
       <c r="D133" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E133">
         <v>4</v>
@@ -3037,7 +2995,7 @@
         <v>26</v>
       </c>
       <c r="D134" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E134">
         <v>5</v>
@@ -3054,7 +3012,7 @@
         <v>27</v>
       </c>
       <c r="D135" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E135">
         <v>6</v>
@@ -3071,7 +3029,7 @@
         <v>27</v>
       </c>
       <c r="D136" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -3088,7 +3046,7 @@
         <v>27</v>
       </c>
       <c r="D137" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E137">
         <v>2</v>
@@ -3105,7 +3063,7 @@
         <v>27</v>
       </c>
       <c r="D138" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E138">
         <v>3</v>
@@ -3292,7 +3250,7 @@
         <v>2</v>
       </c>
       <c r="D149" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="E149">
         <v>3</v>
@@ -3309,7 +3267,7 @@
         <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E150">
         <v>4</v>
@@ -3343,7 +3301,7 @@
         <v>3</v>
       </c>
       <c r="D152" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -3411,7 +3369,7 @@
         <v>4</v>
       </c>
       <c r="D156" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E156">
         <v>1</v>
@@ -3428,7 +3386,7 @@
         <v>4</v>
       </c>
       <c r="D157" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E157">
         <v>2</v>
@@ -3445,7 +3403,7 @@
         <v>4</v>
       </c>
       <c r="D158" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E158">
         <v>3</v>
@@ -3462,7 +3420,7 @@
         <v>4</v>
       </c>
       <c r="D159" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E159">
         <v>4</v>
@@ -3479,7 +3437,7 @@
         <v>4</v>
       </c>
       <c r="D160" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E160">
         <v>5</v>
@@ -3496,7 +3454,7 @@
         <v>4</v>
       </c>
       <c r="D161" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E161">
         <v>6</v>
@@ -3513,7 +3471,7 @@
         <v>4</v>
       </c>
       <c r="D162" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E162">
         <v>7</v>
@@ -3530,7 +3488,7 @@
         <v>5</v>
       </c>
       <c r="D163" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -3547,7 +3505,7 @@
         <v>5</v>
       </c>
       <c r="D164" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E164">
         <v>2</v>
@@ -3564,7 +3522,7 @@
         <v>5</v>
       </c>
       <c r="D165" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E165">
         <v>3</v>
@@ -3581,7 +3539,7 @@
         <v>5</v>
       </c>
       <c r="D166" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E166">
         <v>4</v>
@@ -3598,7 +3556,7 @@
         <v>5</v>
       </c>
       <c r="D167" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E167">
         <v>5</v>
@@ -3615,7 +3573,7 @@
         <v>5</v>
       </c>
       <c r="D168" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E168">
         <v>6</v>
@@ -3632,7 +3590,7 @@
         <v>5</v>
       </c>
       <c r="D169" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E169">
         <v>7</v>
@@ -3700,7 +3658,7 @@
         <v>6</v>
       </c>
       <c r="D173" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E173">
         <v>4</v>
@@ -3819,7 +3777,7 @@
         <v>8</v>
       </c>
       <c r="D180" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -3836,7 +3794,7 @@
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E181">
         <v>2</v>
@@ -3853,7 +3811,7 @@
         <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E182">
         <v>3</v>
@@ -3887,7 +3845,7 @@
         <v>8</v>
       </c>
       <c r="D184" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E184">
         <v>5</v>
@@ -3904,7 +3862,7 @@
         <v>9</v>
       </c>
       <c r="D185" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -3921,7 +3879,7 @@
         <v>9</v>
       </c>
       <c r="D186" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E186">
         <v>2</v>
@@ -3938,7 +3896,7 @@
         <v>9</v>
       </c>
       <c r="D187" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E187">
         <v>3</v>
@@ -3955,7 +3913,7 @@
         <v>9</v>
       </c>
       <c r="D188" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E188">
         <v>4</v>
@@ -3972,7 +3930,7 @@
         <v>9</v>
       </c>
       <c r="D189" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E189">
         <v>5</v>
@@ -4040,7 +3998,7 @@
         <v>10</v>
       </c>
       <c r="D193" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E193">
         <v>4</v>
@@ -4125,7 +4083,7 @@
         <v>11</v>
       </c>
       <c r="D198" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E198">
         <v>3</v>
@@ -4142,7 +4100,7 @@
         <v>11</v>
       </c>
       <c r="D199" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E199">
         <v>4</v>
@@ -4193,7 +4151,7 @@
         <v>12</v>
       </c>
       <c r="D202" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -4210,7 +4168,7 @@
         <v>12</v>
       </c>
       <c r="D203" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E203">
         <v>2</v>
@@ -4227,7 +4185,7 @@
         <v>12</v>
       </c>
       <c r="D204" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E204">
         <v>3</v>
@@ -4244,7 +4202,7 @@
         <v>12</v>
       </c>
       <c r="D205" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E205">
         <v>4</v>
@@ -4261,7 +4219,7 @@
         <v>12</v>
       </c>
       <c r="D206" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E206">
         <v>5</v>
@@ -4278,7 +4236,7 @@
         <v>12</v>
       </c>
       <c r="D207" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E207">
         <v>6</v>
@@ -4312,7 +4270,7 @@
         <v>13</v>
       </c>
       <c r="D209" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E209">
         <v>2</v>
@@ -4958,7 +4916,7 @@
         <v>22</v>
       </c>
       <c r="D247" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -4992,7 +4950,7 @@
         <v>22</v>
       </c>
       <c r="D249" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E249">
         <v>3</v>
@@ -5009,7 +4967,7 @@
         <v>22</v>
       </c>
       <c r="D250" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E250">
         <v>4</v>
@@ -5026,7 +4984,7 @@
         <v>22</v>
       </c>
       <c r="D251" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E251">
         <v>5</v>
@@ -5043,7 +5001,7 @@
         <v>23</v>
       </c>
       <c r="D252" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -5060,7 +5018,7 @@
         <v>23</v>
       </c>
       <c r="D253" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E253">
         <v>2</v>
@@ -5077,7 +5035,7 @@
         <v>23</v>
       </c>
       <c r="D254" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E254">
         <v>3</v>
@@ -5094,7 +5052,7 @@
         <v>23</v>
       </c>
       <c r="D255" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E255">
         <v>4</v>
@@ -5111,7 +5069,7 @@
         <v>23</v>
       </c>
       <c r="D256" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E256">
         <v>5</v>
@@ -5145,7 +5103,7 @@
         <v>24</v>
       </c>
       <c r="D258" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -5162,7 +5120,7 @@
         <v>24</v>
       </c>
       <c r="D259" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E259">
         <v>2</v>
@@ -5179,7 +5137,7 @@
         <v>24</v>
       </c>
       <c r="D260" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E260">
         <v>3</v>
@@ -5196,7 +5154,7 @@
         <v>24</v>
       </c>
       <c r="D261" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E261">
         <v>4</v>
@@ -5213,7 +5171,7 @@
         <v>24</v>
       </c>
       <c r="D262" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E262">
         <v>5</v>
@@ -5400,7 +5358,7 @@
         <v>1</v>
       </c>
       <c r="D273" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E273">
         <v>1</v>
@@ -5417,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="D274" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="E274">
         <v>2</v>
@@ -5434,7 +5392,7 @@
         <v>1</v>
       </c>
       <c r="D275" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="E275">
         <v>3</v>
@@ -5451,7 +5409,7 @@
         <v>1</v>
       </c>
       <c r="D276" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E276">
         <v>4</v>
@@ -5502,7 +5460,7 @@
         <v>2</v>
       </c>
       <c r="D279" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E279">
         <v>2</v>
@@ -5655,7 +5613,7 @@
         <v>4</v>
       </c>
       <c r="D288" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E288">
         <v>1</v>
@@ -5672,7 +5630,7 @@
         <v>4</v>
       </c>
       <c r="D289" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E289">
         <v>2</v>
@@ -5689,7 +5647,7 @@
         <v>4</v>
       </c>
       <c r="D290" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E290">
         <v>3</v>
@@ -5706,7 +5664,7 @@
         <v>4</v>
       </c>
       <c r="D291" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E291">
         <v>4</v>
@@ -5723,7 +5681,7 @@
         <v>4</v>
       </c>
       <c r="D292" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E292">
         <v>5</v>
@@ -5740,7 +5698,7 @@
         <v>4</v>
       </c>
       <c r="D293" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E293">
         <v>6</v>
@@ -5757,7 +5715,7 @@
         <v>4</v>
       </c>
       <c r="D294" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E294">
         <v>7</v>
@@ -5774,7 +5732,7 @@
         <v>4</v>
       </c>
       <c r="D295" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E295">
         <v>8</v>
@@ -5791,7 +5749,7 @@
         <v>5</v>
       </c>
       <c r="D296" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E296">
         <v>1</v>
@@ -5808,7 +5766,7 @@
         <v>5</v>
       </c>
       <c r="D297" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E297">
         <v>2</v>
@@ -5825,7 +5783,7 @@
         <v>5</v>
       </c>
       <c r="D298" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E298">
         <v>3</v>
@@ -5842,7 +5800,7 @@
         <v>5</v>
       </c>
       <c r="D299" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="E299">
         <v>4</v>
@@ -5859,7 +5817,7 @@
         <v>5</v>
       </c>
       <c r="D300" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E300">
         <v>5</v>
@@ -5876,7 +5834,7 @@
         <v>5</v>
       </c>
       <c r="D301" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="E301">
         <v>6</v>
@@ -6046,7 +6004,7 @@
         <v>7</v>
       </c>
       <c r="D311" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E311">
         <v>6</v>
@@ -6063,7 +6021,7 @@
         <v>8</v>
       </c>
       <c r="D312" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E312">
         <v>1</v>
@@ -6080,7 +6038,7 @@
         <v>8</v>
       </c>
       <c r="D313" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E313">
         <v>2</v>
@@ -6097,7 +6055,7 @@
         <v>8</v>
       </c>
       <c r="D314" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E314">
         <v>3</v>
@@ -6114,7 +6072,7 @@
         <v>8</v>
       </c>
       <c r="D315" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E315">
         <v>4</v>
@@ -6131,7 +6089,7 @@
         <v>8</v>
       </c>
       <c r="D316" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E316">
         <v>5</v>
@@ -6148,7 +6106,7 @@
         <v>9</v>
       </c>
       <c r="D317" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E317">
         <v>1</v>
@@ -6182,7 +6140,7 @@
         <v>9</v>
       </c>
       <c r="D319" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E319">
         <v>3</v>
@@ -6199,7 +6157,7 @@
         <v>9</v>
       </c>
       <c r="D320" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E320">
         <v>4</v>
@@ -6216,7 +6174,7 @@
         <v>9</v>
       </c>
       <c r="D321" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E321">
         <v>5</v>
@@ -6267,7 +6225,7 @@
         <v>10</v>
       </c>
       <c r="D324" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="E324">
         <v>3</v>
@@ -6335,7 +6293,7 @@
         <v>11</v>
       </c>
       <c r="D328" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E328">
         <v>1</v>
@@ -6352,7 +6310,7 @@
         <v>11</v>
       </c>
       <c r="D329" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E329">
         <v>2</v>
@@ -6369,7 +6327,7 @@
         <v>11</v>
       </c>
       <c r="D330" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E330">
         <v>3</v>
@@ -6386,7 +6344,7 @@
         <v>11</v>
       </c>
       <c r="D331" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E331">
         <v>4</v>
@@ -6403,7 +6361,7 @@
         <v>11</v>
       </c>
       <c r="D332" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E332">
         <v>5</v>
@@ -6420,7 +6378,7 @@
         <v>11</v>
       </c>
       <c r="D333" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E333">
         <v>6</v>
@@ -6488,7 +6446,7 @@
         <v>13</v>
       </c>
       <c r="D337" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E337">
         <v>1</v>
@@ -6522,7 +6480,7 @@
         <v>13</v>
       </c>
       <c r="D339" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E339">
         <v>3</v>
@@ -6539,7 +6497,7 @@
         <v>13</v>
       </c>
       <c r="D340" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E340">
         <v>4</v>
@@ -7202,7 +7160,7 @@
         <v>22</v>
       </c>
       <c r="D379" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E379">
         <v>1</v>
@@ -7219,7 +7177,7 @@
         <v>22</v>
       </c>
       <c r="D380" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E380">
         <v>2</v>
@@ -7236,7 +7194,7 @@
         <v>22</v>
       </c>
       <c r="D381" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E381">
         <v>3</v>
@@ -7253,7 +7211,7 @@
         <v>22</v>
       </c>
       <c r="D382" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E382">
         <v>4</v>
@@ -7270,7 +7228,7 @@
         <v>22</v>
       </c>
       <c r="D383" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E383">
         <v>5</v>
@@ -7287,7 +7245,7 @@
         <v>23</v>
       </c>
       <c r="D384" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E384">
         <v>1</v>
@@ -7304,7 +7262,7 @@
         <v>23</v>
       </c>
       <c r="D385" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E385">
         <v>2</v>
@@ -7321,7 +7279,7 @@
         <v>23</v>
       </c>
       <c r="D386" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E386">
         <v>3</v>
@@ -7338,7 +7296,7 @@
         <v>23</v>
       </c>
       <c r="D387" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E387">
         <v>4</v>
@@ -7355,7 +7313,7 @@
         <v>23</v>
       </c>
       <c r="D388" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E388">
         <v>5</v>
@@ -7542,7 +7500,7 @@
         <v>26</v>
       </c>
       <c r="D399" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E399">
         <v>1</v>
@@ -7559,7 +7517,7 @@
         <v>26</v>
       </c>
       <c r="D400" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E400">
         <v>2</v>
@@ -7576,7 +7534,7 @@
         <v>26</v>
       </c>
       <c r="D401" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E401">
         <v>3</v>
@@ -7593,7 +7551,7 @@
         <v>26</v>
       </c>
       <c r="D402" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E402">
         <v>4</v>
@@ -7610,7 +7568,7 @@
         <v>26</v>
       </c>
       <c r="D403" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E403">
         <v>5</v>
@@ -7644,7 +7602,7 @@
         <v>27</v>
       </c>
       <c r="D405" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E405">
         <v>1</v>
@@ -7661,7 +7619,7 @@
         <v>27</v>
       </c>
       <c r="D406" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E406">
         <v>2</v>
@@ -7678,7 +7636,7 @@
         <v>27</v>
       </c>
       <c r="D407" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E407">
         <v>3</v>
@@ -7695,7 +7653,7 @@
         <v>27</v>
       </c>
       <c r="D408" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E408">
         <v>4</v>
@@ -7712,7 +7670,7 @@
         <v>27</v>
       </c>
       <c r="D409" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E409">
         <v>5</v>
@@ -7729,7 +7687,7 @@
         <v>1</v>
       </c>
       <c r="D410" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E410">
         <v>1</v>
@@ -7848,7 +7806,7 @@
         <v>2</v>
       </c>
       <c r="D417" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E417">
         <v>2</v>
@@ -7967,7 +7925,7 @@
         <v>3</v>
       </c>
       <c r="D424" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E424">
         <v>4</v>
@@ -7984,7 +7942,7 @@
         <v>4</v>
       </c>
       <c r="D425" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E425">
         <v>1</v>
@@ -8001,7 +7959,7 @@
         <v>4</v>
       </c>
       <c r="D426" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E426">
         <v>2</v>
@@ -8018,7 +7976,7 @@
         <v>4</v>
       </c>
       <c r="D427" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E427">
         <v>3</v>
@@ -8035,7 +7993,7 @@
         <v>4</v>
       </c>
       <c r="D428" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="E428">
         <v>4</v>
@@ -8052,7 +8010,7 @@
         <v>4</v>
       </c>
       <c r="D429" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E429">
         <v>5</v>
@@ -8069,7 +8027,7 @@
         <v>4</v>
       </c>
       <c r="D430" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E430">
         <v>6</v>
@@ -8086,7 +8044,7 @@
         <v>4</v>
       </c>
       <c r="D431" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E431">
         <v>7</v>
@@ -8103,7 +8061,7 @@
         <v>5</v>
       </c>
       <c r="D432" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E432">
         <v>1</v>
@@ -8120,7 +8078,7 @@
         <v>5</v>
       </c>
       <c r="D433" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E433">
         <v>2</v>
@@ -8137,7 +8095,7 @@
         <v>5</v>
       </c>
       <c r="D434" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E434">
         <v>3</v>
@@ -8154,7 +8112,7 @@
         <v>5</v>
       </c>
       <c r="D435" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E435">
         <v>4</v>
@@ -8171,7 +8129,7 @@
         <v>5</v>
       </c>
       <c r="D436" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E436">
         <v>5</v>
@@ -8188,7 +8146,7 @@
         <v>5</v>
       </c>
       <c r="D437" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E437">
         <v>6</v>
@@ -8205,7 +8163,7 @@
         <v>5</v>
       </c>
       <c r="D438" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E438">
         <v>7</v>
@@ -8222,7 +8180,7 @@
         <v>6</v>
       </c>
       <c r="D439" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E439">
         <v>1</v>
@@ -8239,7 +8197,7 @@
         <v>6</v>
       </c>
       <c r="D440" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E440">
         <v>2</v>
@@ -8256,7 +8214,7 @@
         <v>6</v>
       </c>
       <c r="D441" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E441">
         <v>3</v>
@@ -8273,7 +8231,7 @@
         <v>6</v>
       </c>
       <c r="D442" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E442">
         <v>4</v>
@@ -8375,7 +8333,7 @@
         <v>7</v>
       </c>
       <c r="D448" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E448">
         <v>4</v>
@@ -8426,7 +8384,7 @@
         <v>8</v>
       </c>
       <c r="D451" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E451">
         <v>3</v>
@@ -8494,7 +8452,7 @@
         <v>9</v>
       </c>
       <c r="D455" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E455">
         <v>1</v>
@@ -8511,7 +8469,7 @@
         <v>9</v>
       </c>
       <c r="D456" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E456">
         <v>2</v>
@@ -8528,7 +8486,7 @@
         <v>9</v>
       </c>
       <c r="D457" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E457">
         <v>3</v>
@@ -8545,7 +8503,7 @@
         <v>9</v>
       </c>
       <c r="D458" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E458">
         <v>4</v>
@@ -8613,7 +8571,7 @@
         <v>11</v>
       </c>
       <c r="D462" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E462">
         <v>1</v>
@@ -8647,7 +8605,7 @@
         <v>11</v>
       </c>
       <c r="D464" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E464">
         <v>3</v>
@@ -8664,7 +8622,7 @@
         <v>11</v>
       </c>
       <c r="D465" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E465">
         <v>4</v>
@@ -8681,7 +8639,7 @@
         <v>11</v>
       </c>
       <c r="D466" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E466">
         <v>5</v>
@@ -8698,7 +8656,7 @@
         <v>11</v>
       </c>
       <c r="D467" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E467">
         <v>6</v>
@@ -8749,7 +8707,7 @@
         <v>12</v>
       </c>
       <c r="D470" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E470">
         <v>3</v>
@@ -8834,7 +8792,7 @@
         <v>13</v>
       </c>
       <c r="D475" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E475">
         <v>2</v>
@@ -8851,7 +8809,7 @@
         <v>13</v>
       </c>
       <c r="D476" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E476">
         <v>3</v>
@@ -8868,7 +8826,7 @@
         <v>13</v>
       </c>
       <c r="D477" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E477">
         <v>4</v>
@@ -8885,7 +8843,7 @@
         <v>13</v>
       </c>
       <c r="D478" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E478">
         <v>5</v>
@@ -9361,7 +9319,7 @@
         <v>20</v>
       </c>
       <c r="D506" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E506">
         <v>1</v>
@@ -9378,7 +9336,7 @@
         <v>20</v>
       </c>
       <c r="D507" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E507">
         <v>2</v>
@@ -9395,7 +9353,7 @@
         <v>20</v>
       </c>
       <c r="D508" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E508">
         <v>3</v>
@@ -9412,7 +9370,7 @@
         <v>20</v>
       </c>
       <c r="D509" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E509">
         <v>4</v>
@@ -9429,7 +9387,7 @@
         <v>20</v>
       </c>
       <c r="D510" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E510">
         <v>5</v>
@@ -9446,7 +9404,7 @@
         <v>21</v>
       </c>
       <c r="D511" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E511">
         <v>1</v>
@@ -9463,7 +9421,7 @@
         <v>21</v>
       </c>
       <c r="D512" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E512">
         <v>2</v>
@@ -9480,7 +9438,7 @@
         <v>21</v>
       </c>
       <c r="D513" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E513">
         <v>3</v>
@@ -9497,7 +9455,7 @@
         <v>21</v>
       </c>
       <c r="D514" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E514">
         <v>4</v>
@@ -9514,13 +9472,13 @@
         <v>21</v>
       </c>
       <c r="D515" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E515">
         <v>5</v>
       </c>
       <c r="F515" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="516" spans="1:6" x14ac:dyDescent="0.2">
@@ -9795,7 +9753,7 @@
         <v>6</v>
       </c>
       <c r="F531" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="532" spans="1:6" x14ac:dyDescent="0.2">
@@ -9894,7 +9852,7 @@
         <v>26</v>
       </c>
       <c r="D537" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E537">
         <v>1</v>
@@ -9911,7 +9869,7 @@
         <v>26</v>
       </c>
       <c r="D538" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E538">
         <v>2</v>
@@ -9928,7 +9886,7 @@
         <v>26</v>
       </c>
       <c r="D539" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E539">
         <v>3</v>
@@ -9945,7 +9903,7 @@
         <v>26</v>
       </c>
       <c r="D540" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E540">
         <v>4</v>
@@ -9962,7 +9920,7 @@
         <v>26</v>
       </c>
       <c r="D541" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E541">
         <v>5</v>
@@ -9979,7 +9937,7 @@
         <v>27</v>
       </c>
       <c r="D542" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E542">
         <v>1</v>
@@ -9996,7 +9954,7 @@
         <v>27</v>
       </c>
       <c r="D543" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E543">
         <v>2</v>
@@ -10013,7 +9971,7 @@
         <v>27</v>
       </c>
       <c r="D544" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E544">
         <v>3</v>
@@ -10030,7 +9988,7 @@
         <v>27</v>
       </c>
       <c r="D545" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E545">
         <v>4</v>
@@ -10047,7 +10005,7 @@
         <v>27</v>
       </c>
       <c r="D546" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E546">
         <v>5</v>
@@ -10081,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="D548" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E548">
         <v>2</v>
@@ -10115,7 +10073,7 @@
         <v>1</v>
       </c>
       <c r="D550" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E550">
         <v>4</v>
@@ -10183,7 +10141,7 @@
         <v>2</v>
       </c>
       <c r="D554" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E554">
         <v>3</v>
@@ -10251,7 +10209,7 @@
         <v>3</v>
       </c>
       <c r="D558" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E558">
         <v>1</v>
@@ -10336,7 +10294,7 @@
         <v>4</v>
       </c>
       <c r="D563" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E563">
         <v>1</v>
@@ -10353,7 +10311,7 @@
         <v>4</v>
       </c>
       <c r="D564" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E564">
         <v>2</v>
@@ -10370,7 +10328,7 @@
         <v>4</v>
       </c>
       <c r="D565" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E565">
         <v>3</v>
@@ -10387,7 +10345,7 @@
         <v>4</v>
       </c>
       <c r="D566" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E566">
         <v>4</v>
@@ -10404,7 +10362,7 @@
         <v>4</v>
       </c>
       <c r="D567" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E567">
         <v>5</v>
@@ -10421,7 +10379,7 @@
         <v>4</v>
       </c>
       <c r="D568" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E568">
         <v>6</v>
@@ -10438,7 +10396,7 @@
         <v>4</v>
       </c>
       <c r="D569" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E569">
         <v>7</v>
@@ -10455,7 +10413,7 @@
         <v>5</v>
       </c>
       <c r="D570" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E570">
         <v>1</v>
@@ -10472,7 +10430,7 @@
         <v>5</v>
       </c>
       <c r="D571" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E571">
         <v>2</v>
@@ -10489,7 +10447,7 @@
         <v>5</v>
       </c>
       <c r="D572" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E572">
         <v>3</v>
@@ -10506,7 +10464,7 @@
         <v>5</v>
       </c>
       <c r="D573" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E573">
         <v>4</v>
@@ -10523,7 +10481,7 @@
         <v>5</v>
       </c>
       <c r="D574" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E574">
         <v>5</v>
@@ -10540,7 +10498,7 @@
         <v>5</v>
       </c>
       <c r="D575" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E575">
         <v>6</v>
@@ -10557,7 +10515,7 @@
         <v>5</v>
       </c>
       <c r="D576" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E576">
         <v>7</v>
@@ -10608,7 +10566,7 @@
         <v>6</v>
       </c>
       <c r="D579" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E579">
         <v>3</v>
@@ -10659,7 +10617,7 @@
         <v>7</v>
       </c>
       <c r="D582" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E582">
         <v>1</v>
@@ -10693,7 +10651,7 @@
         <v>7</v>
       </c>
       <c r="D584" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E584">
         <v>3</v>
@@ -10727,7 +10685,7 @@
         <v>7</v>
       </c>
       <c r="D586" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E586">
         <v>5</v>
@@ -10744,7 +10702,7 @@
         <v>8</v>
       </c>
       <c r="D587" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E587">
         <v>1</v>
@@ -10761,7 +10719,7 @@
         <v>8</v>
       </c>
       <c r="D588" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E588">
         <v>2</v>
@@ -10778,7 +10736,7 @@
         <v>8</v>
       </c>
       <c r="D589" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E589">
         <v>3</v>
@@ -10795,7 +10753,7 @@
         <v>8</v>
       </c>
       <c r="D590" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E590">
         <v>4</v>
@@ -10812,7 +10770,7 @@
         <v>8</v>
       </c>
       <c r="D591" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E591">
         <v>5</v>
@@ -10897,7 +10855,7 @@
         <v>9</v>
       </c>
       <c r="D596" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E596">
         <v>5</v>
@@ -10999,7 +10957,7 @@
         <v>10</v>
       </c>
       <c r="D602" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E602">
         <v>6</v>
@@ -11016,7 +10974,7 @@
         <v>11</v>
       </c>
       <c r="D603" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E603">
         <v>1</v>
@@ -11033,7 +10991,7 @@
         <v>11</v>
       </c>
       <c r="D604" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E604">
         <v>2</v>
@@ -11050,7 +11008,7 @@
         <v>11</v>
       </c>
       <c r="D605" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E605">
         <v>3</v>
@@ -11067,7 +11025,7 @@
         <v>11</v>
       </c>
       <c r="D606" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E606">
         <v>4</v>
@@ -11084,7 +11042,7 @@
         <v>11</v>
       </c>
       <c r="D607" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E607">
         <v>5</v>
@@ -11101,7 +11059,7 @@
         <v>11</v>
       </c>
       <c r="D608" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E608">
         <v>6</v>
@@ -11118,7 +11076,7 @@
         <v>12</v>
       </c>
       <c r="D609" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E609">
         <v>1</v>
@@ -11135,7 +11093,7 @@
         <v>12</v>
       </c>
       <c r="D610" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E610">
         <v>2</v>
@@ -11169,7 +11127,7 @@
         <v>12</v>
       </c>
       <c r="D612" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E612">
         <v>4</v>
@@ -11424,7 +11382,7 @@
         <v>16</v>
       </c>
       <c r="D627" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E627">
         <v>1</v>
@@ -11441,7 +11399,7 @@
         <v>16</v>
       </c>
       <c r="D628" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E628">
         <v>2</v>
@@ -11458,7 +11416,7 @@
         <v>16</v>
       </c>
       <c r="D629" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E629">
         <v>3</v>
@@ -11475,7 +11433,7 @@
         <v>16</v>
       </c>
       <c r="D630" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E630">
         <v>4</v>
@@ -11492,7 +11450,7 @@
         <v>16</v>
       </c>
       <c r="D631" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E631">
         <v>5</v>
@@ -11509,7 +11467,7 @@
         <v>17</v>
       </c>
       <c r="D632" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E632">
         <v>1</v>
@@ -11526,7 +11484,7 @@
         <v>17</v>
       </c>
       <c r="D633" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E633">
         <v>2</v>
@@ -11543,7 +11501,7 @@
         <v>17</v>
       </c>
       <c r="D634" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E634">
         <v>3</v>
@@ -11560,7 +11518,7 @@
         <v>17</v>
       </c>
       <c r="D635" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E635">
         <v>4</v>
@@ -11577,7 +11535,7 @@
         <v>17</v>
       </c>
       <c r="D636" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E636">
         <v>5</v>
@@ -11594,7 +11552,7 @@
         <v>18</v>
       </c>
       <c r="D637" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E637">
         <v>1</v>
@@ -11611,7 +11569,7 @@
         <v>18</v>
       </c>
       <c r="D638" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E638">
         <v>2</v>
@@ -11628,7 +11586,7 @@
         <v>18</v>
       </c>
       <c r="D639" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E639">
         <v>3</v>
@@ -11645,7 +11603,7 @@
         <v>18</v>
       </c>
       <c r="D640" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E640">
         <v>4</v>
@@ -11662,7 +11620,7 @@
         <v>18</v>
       </c>
       <c r="D641" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E641">
         <v>5</v>
@@ -11679,7 +11637,7 @@
         <v>19</v>
       </c>
       <c r="D642" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E642">
         <v>1</v>
@@ -11696,7 +11654,7 @@
         <v>19</v>
       </c>
       <c r="D643" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E643">
         <v>2</v>
@@ -11713,7 +11671,7 @@
         <v>19</v>
       </c>
       <c r="D644" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E644">
         <v>3</v>
@@ -11730,7 +11688,7 @@
         <v>19</v>
       </c>
       <c r="D645" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E645">
         <v>4</v>
@@ -11747,7 +11705,7 @@
         <v>19</v>
       </c>
       <c r="D646" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E646">
         <v>5</v>

</xml_diff>